<commit_message>
Image OD and Seg file update
</commit_message>
<xml_diff>
--- a/object_detection_Wheat/Experiments_ObjectDetection.xlsx
+++ b/object_detection_Wheat/Experiments_ObjectDetection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YShimada-MBP16/Documents/Code_Github/DL_for_ImageData_and_Finetuning/object_detection_Wheat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CD095E-9656-E54D-A29D-6C8257ECDDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7B203A-AD89-CD4F-8653-B712D8BE902A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39840" yWindow="2200" windowWidth="27160" windowHeight="17120" xr2:uid="{29C2A13E-54B7-0448-97D9-C07A7F20C391}"/>
   </bookViews>
@@ -146,10 +146,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Validation mAP</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Status</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -245,6 +241,10 @@
   </si>
   <si>
     <t>name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Validation mAP@0.5</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -758,7 +758,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E4"/>
+      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -769,19 +769,19 @@
   <sheetData>
     <row r="1" spans="1:11" ht="63">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>8</v>
@@ -793,10 +793,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J1" s="13" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="K1" s="14" t="s">
         <v>7</v>
@@ -807,10 +807,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="5">
         <v>25.56</v>
@@ -842,10 +842,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>25.56</v>
@@ -874,13 +874,13 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>25.56</v>
@@ -909,13 +909,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>24.14</v>
@@ -947,10 +947,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>24.14</v>
@@ -982,10 +982,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>24.14</v>
@@ -1014,13 +1014,13 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>23.37</v>
@@ -1052,10 +1052,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>23.37</v>
@@ -1087,10 +1087,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="10">
         <v>23.37</v>
@@ -1119,13 +1119,13 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>25.56</v>
@@ -1157,10 +1157,10 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>25.56</v>
@@ -1192,10 +1192,10 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13">
         <v>25.56</v>
@@ -1227,10 +1227,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>24.14</v>
@@ -1257,13 +1257,13 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
       </c>
       <c r="D15">
         <v>24.14</v>
@@ -1295,10 +1295,10 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>24.14</v>
@@ -1327,13 +1327,13 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>41</v>
       </c>
       <c r="D17">
         <v>23.37</v>
@@ -1365,10 +1365,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>23.37</v>
@@ -1400,10 +1400,10 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19">
         <v>23.37</v>
@@ -1435,7 +1435,7 @@
         <v>21</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>29</v>
@@ -1470,7 +1470,7 @@
         <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
         <v>29</v>
@@ -1505,7 +1505,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>29</v>
@@ -1537,13 +1537,13 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23">
         <v>24.3</v>
@@ -1572,13 +1572,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24">
         <v>24.3</v>
@@ -1607,13 +1607,13 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25">
         <v>24.3</v>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26">
         <v>20.7</v>
@@ -1677,13 +1677,13 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27">
         <v>20.7</v>
@@ -1712,13 +1712,13 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="D28" s="10">
         <v>20.7</v>
@@ -1789,7 +1789,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C65085E-90E8-3347-9881-3515951A7E55}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
@@ -1800,19 +1802,19 @@
   <sheetData>
     <row r="1" spans="1:13" ht="63">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -1824,10 +1826,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>7</v>
@@ -1838,10 +1840,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>25.56</v>
@@ -1875,10 +1877,10 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>25.56</v>
@@ -1909,13 +1911,13 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>25.56</v>
@@ -1946,13 +1948,13 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>24.14</v>
@@ -1986,10 +1988,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>24.14</v>
@@ -2023,10 +2025,10 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>24.14</v>
@@ -2057,13 +2059,13 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>23.37</v>
@@ -2097,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>23.37</v>
@@ -2134,10 +2136,10 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>23.37</v>
@@ -2181,7 +2183,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C0389E-E471-274B-A009-102A7F5D751D}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
@@ -2192,19 +2196,19 @@
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1" ht="63">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -2216,10 +2220,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>7</v>
@@ -2227,13 +2231,13 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>25.56</v>
@@ -2267,10 +2271,10 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3">
         <v>25.56</v>
@@ -2304,10 +2308,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4">
         <v>25.56</v>
@@ -2341,10 +2345,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>24.14</v>
@@ -2372,13 +2376,13 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>38</v>
       </c>
       <c r="D6">
         <v>24.14</v>
@@ -2412,10 +2416,10 @@
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>24.14</v>
@@ -2446,13 +2450,13 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
       </c>
       <c r="D8">
         <v>23.37</v>
@@ -2486,10 +2490,10 @@
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>23.37</v>
@@ -2521,10 +2525,10 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>23.37</v>
@@ -2569,7 +2573,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -2583,19 +2587,19 @@
   <sheetData>
     <row r="1" spans="1:16" s="3" customFormat="1" ht="42">
       <c r="A1" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>8</v>
@@ -2607,10 +2611,10 @@
         <v>10</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>30</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>7</v>
@@ -2621,7 +2625,7 @@
         <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -2656,7 +2660,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -2695,7 +2699,7 @@
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -2731,13 +2735,13 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5">
         <v>24.3</v>
@@ -2770,13 +2774,13 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>24.3</v>
@@ -2805,13 +2809,13 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7">
         <v>24.3</v>
@@ -2844,13 +2848,13 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8">
         <v>20.7</v>
@@ -2879,13 +2883,13 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <v>20.7</v>
@@ -2918,13 +2922,13 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
       </c>
       <c r="D10">
         <v>20.7</v>
@@ -2960,7 +2964,7 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -2990,7 +2994,7 @@
         <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>25</v>
@@ -3021,7 +3025,7 @@
         <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
@@ -3051,7 +3055,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -3086,7 +3090,7 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -3121,7 +3125,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>

</xml_diff>